<commit_message>
added another DC text
</commit_message>
<xml_diff>
--- a/03. Microprocessors & Microcontrollers/8086.xlsx
+++ b/03. Microprocessors & Microcontrollers/8086.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srivi\Documents\COLLEGE STUFF\ACADEMICS\S5\03. Microprocessors &amp; Microcontrollers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4265E035-D693-4641-84E9-D8264F45577C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DE6680-845E-42B0-9026-3C9B14EAE378}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E476FC97-EF1C-4CFF-BA19-101056E77814}"/>
   </bookViews>
@@ -1533,7 +1533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1733,9 +1733,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1781,26 +1778,230 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1808,206 +2009,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2325,9 +2358,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D51FDA2-F68B-4259-B27A-3AE6B6ABB098}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2376,45 +2409,45 @@
       <c r="B2" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="70" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="23"/>
-      <c r="E2" s="70" t="s">
+      <c r="E2" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="F2" s="154" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="69" t="s">
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="68" t="s">
+      <c r="K2" s="67" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="92" t="s">
+    <row r="3" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="127" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="139" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="65"/>
-      <c r="E3" s="86" t="s">
+      <c r="E3" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="151" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="157"/>
+      <c r="I3" s="163"/>
       <c r="J3" s="45"/>
-      <c r="K3" s="145" t="s">
+      <c r="K3" s="167" t="s">
         <v>25</v>
       </c>
       <c r="M3" s="7" t="s">
@@ -2428,16 +2461,16 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B4" s="92"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="146"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="132"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="150"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="159"/>
+      <c r="H4" s="159"/>
+      <c r="I4" s="164"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="168"/>
       <c r="M4" s="11">
         <v>0</v>
       </c>
@@ -2449,18 +2482,18 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B5" s="92"/>
-      <c r="C5" s="61" t="s">
+      <c r="B5" s="127"/>
+      <c r="C5" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="26"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="150"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="159"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="164"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="168"/>
       <c r="M5" s="13">
         <v>0</v>
       </c>
@@ -2472,18 +2505,18 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B6" s="92"/>
+      <c r="B6" s="127"/>
       <c r="C6" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="26"/>
+      <c r="D6" s="160"/>
+      <c r="E6" s="150"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="159"/>
+      <c r="H6" s="159"/>
+      <c r="I6" s="164"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="168"/>
       <c r="M6" s="13">
         <v>1</v>
       </c>
@@ -2495,18 +2528,18 @@
       </c>
     </row>
     <row r="7" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="92"/>
+      <c r="B7" s="127"/>
       <c r="C7" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="26"/>
+      <c r="D7" s="160"/>
+      <c r="E7" s="150"/>
+      <c r="F7" s="152"/>
+      <c r="G7" s="159"/>
+      <c r="H7" s="159"/>
+      <c r="I7" s="164"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="168"/>
       <c r="M7" s="8">
         <v>1</v>
       </c>
@@ -2518,55 +2551,55 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B8" s="92"/>
-      <c r="C8" s="110" t="s">
+      <c r="B8" s="127"/>
+      <c r="C8" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="26"/>
+      <c r="D8" s="161"/>
+      <c r="E8" s="150"/>
+      <c r="F8" s="152"/>
+      <c r="G8" s="159"/>
+      <c r="H8" s="159"/>
+      <c r="I8" s="164"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="168"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
     </row>
     <row r="9" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="92"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="52"/>
+      <c r="B9" s="127"/>
+      <c r="C9" s="133"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="165"/>
+      <c r="G9" s="158"/>
+      <c r="H9" s="158"/>
+      <c r="I9" s="166"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="169"/>
     </row>
     <row r="10" spans="2:18" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="128" t="s">
         <v>100</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="39"/>
-      <c r="E10" s="106" t="s">
+      <c r="E10" s="151" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="93" t="s">
+      <c r="F10" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="94"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86" t="s">
+      <c r="G10" s="146"/>
+      <c r="H10" s="131"/>
+      <c r="I10" s="131" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="95" t="s">
+      <c r="J10" s="140" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="100" t="s">
+      <c r="K10" s="129" t="s">
         <v>38</v>
       </c>
       <c r="M10" s="16" t="s">
@@ -2575,49 +2608,49 @@
       <c r="N10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="153" t="s">
+      <c r="O10" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="154"/>
-      <c r="Q10" s="155"/>
+      <c r="P10" s="103"/>
+      <c r="Q10" s="104"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B11" s="103"/>
+      <c r="B11" s="128"/>
       <c r="C11" s="61"/>
       <c r="D11" s="25"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="108"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="105"/>
-      <c r="I11" s="105"/>
-      <c r="J11" s="99"/>
-      <c r="K11" s="101"/>
+      <c r="E11" s="152"/>
+      <c r="F11" s="153"/>
+      <c r="G11" s="100"/>
+      <c r="H11" s="150"/>
+      <c r="I11" s="150"/>
+      <c r="J11" s="136"/>
+      <c r="K11" s="135"/>
       <c r="M11" s="11">
         <v>0</v>
       </c>
       <c r="N11" s="12">
         <v>0</v>
       </c>
-      <c r="O11" s="122" t="s">
+      <c r="O11" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="P11" s="109"/>
-      <c r="Q11" s="123"/>
+      <c r="P11" s="100"/>
+      <c r="Q11" s="101"/>
       <c r="R11" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B12" s="103"/>
+      <c r="B12" s="128"/>
       <c r="C12" s="61"/>
       <c r="D12" s="61"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="108"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="105"/>
-      <c r="I12" s="105"/>
-      <c r="J12" s="99"/>
-      <c r="K12" s="101"/>
+      <c r="E12" s="152"/>
+      <c r="F12" s="153"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="150"/>
+      <c r="I12" s="150"/>
+      <c r="J12" s="136"/>
+      <c r="K12" s="135"/>
       <c r="M12" s="13"/>
       <c r="N12" s="12"/>
       <c r="O12" s="13"/>
@@ -2625,50 +2658,50 @@
       <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B13" s="103"/>
+      <c r="B13" s="128"/>
       <c r="C13" s="60"/>
       <c r="D13" s="25"/>
-      <c r="E13" s="107"/>
-      <c r="F13" s="96"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="98"/>
-      <c r="K13" s="102"/>
+      <c r="E13" s="152"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="148"/>
+      <c r="H13" s="114"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="141"/>
+      <c r="K13" s="130"/>
       <c r="M13" s="13">
         <v>0</v>
       </c>
       <c r="N13" s="12">
         <v>1</v>
       </c>
-      <c r="O13" s="122" t="s">
+      <c r="O13" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="P13" s="109"/>
-      <c r="Q13" s="123"/>
+      <c r="P13" s="100"/>
+      <c r="Q13" s="101"/>
       <c r="R13" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="149" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="88" t="s">
+      <c r="C14" s="139" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="33"/>
       <c r="E14" s="37"/>
-      <c r="F14" s="93" t="s">
+      <c r="F14" s="145" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="94"/>
-      <c r="H14" s="95"/>
+      <c r="G14" s="146"/>
+      <c r="H14" s="140"/>
       <c r="I14" s="45"/>
-      <c r="J14" s="95" t="s">
+      <c r="J14" s="140" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="112" t="s">
+      <c r="K14" s="137" t="s">
         <v>41</v>
       </c>
       <c r="M14" s="13">
@@ -2677,43 +2710,43 @@
       <c r="N14" s="12">
         <v>0</v>
       </c>
-      <c r="O14" s="122" t="s">
+      <c r="O14" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="P14" s="109"/>
-      <c r="Q14" s="123"/>
+      <c r="P14" s="100"/>
+      <c r="Q14" s="101"/>
       <c r="R14" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="104"/>
-      <c r="C15" s="89"/>
+      <c r="B15" s="149"/>
+      <c r="C15" s="133"/>
       <c r="D15" s="66"/>
       <c r="E15" s="38"/>
-      <c r="F15" s="96"/>
-      <c r="G15" s="97"/>
-      <c r="H15" s="98"/>
+      <c r="F15" s="147"/>
+      <c r="G15" s="148"/>
+      <c r="H15" s="141"/>
       <c r="I15" s="46"/>
-      <c r="J15" s="98"/>
-      <c r="K15" s="113"/>
+      <c r="J15" s="141"/>
+      <c r="K15" s="138"/>
       <c r="M15" s="8">
         <v>1</v>
       </c>
       <c r="N15" s="9">
         <v>1</v>
       </c>
-      <c r="O15" s="142" t="s">
+      <c r="O15" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="P15" s="143"/>
-      <c r="Q15" s="144"/>
+      <c r="P15" s="88"/>
+      <c r="Q15" s="89"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B16" s="103" t="s">
+      <c r="B16" s="128" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="88" t="s">
+      <c r="C16" s="139" t="s">
         <v>43</v>
       </c>
       <c r="D16" s="33"/>
@@ -2722,27 +2755,27 @@
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="54"/>
-      <c r="J16" s="95" t="s">
+      <c r="J16" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="114" t="s">
+      <c r="K16" s="142" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B17" s="103"/>
-      <c r="C17" s="89"/>
+      <c r="B17" s="128"/>
+      <c r="C17" s="133"/>
       <c r="D17" s="66"/>
       <c r="E17" s="38"/>
       <c r="F17" s="38"/>
       <c r="G17" s="38"/>
       <c r="H17" s="38"/>
       <c r="I17" s="46"/>
-      <c r="J17" s="98"/>
-      <c r="K17" s="113"/>
+      <c r="J17" s="141"/>
+      <c r="K17" s="138"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B18" s="103" t="s">
+      <c r="B18" s="128" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="61" t="s">
@@ -2754,16 +2787,16 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="54"/>
-      <c r="J18" s="115" t="s">
+      <c r="J18" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="112" t="s">
+      <c r="K18" s="137" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B19" s="103"/>
-      <c r="C19" s="110" t="s">
+      <c r="B19" s="128"/>
+      <c r="C19" s="132" t="s">
         <v>49</v>
       </c>
       <c r="D19" s="33"/>
@@ -2772,23 +2805,23 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="54"/>
-      <c r="J19" s="116"/>
-      <c r="K19" s="112"/>
+      <c r="J19" s="144"/>
+      <c r="K19" s="137"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B20" s="103"/>
-      <c r="C20" s="110"/>
+      <c r="B20" s="128"/>
+      <c r="C20" s="132"/>
       <c r="D20" s="33"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="54"/>
-      <c r="J20" s="117"/>
-      <c r="K20" s="112"/>
+      <c r="J20" s="119"/>
+      <c r="K20" s="137"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="128" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="59" t="s">
@@ -2800,13 +2833,13 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="54"/>
-      <c r="J21" s="99"/>
-      <c r="K21" s="100" t="s">
+      <c r="J21" s="136"/>
+      <c r="K21" s="129" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B22" s="103"/>
+      <c r="B22" s="128"/>
       <c r="C22" s="60" t="s">
         <v>52</v>
       </c>
@@ -2816,11 +2849,11 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="54"/>
-      <c r="J22" s="99"/>
-      <c r="K22" s="101"/>
+      <c r="J22" s="136"/>
+      <c r="K22" s="135"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B23" s="103" t="s">
+      <c r="B23" s="128" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="61" t="s">
@@ -2833,12 +2866,12 @@
       <c r="H23" s="10"/>
       <c r="I23" s="54"/>
       <c r="J23" s="54"/>
-      <c r="K23" s="100" t="s">
+      <c r="K23" s="129" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B24" s="103"/>
+      <c r="B24" s="128"/>
       <c r="C24" s="61" t="s">
         <v>55</v>
       </c>
@@ -2849,10 +2882,10 @@
       <c r="H24" s="10"/>
       <c r="I24" s="54"/>
       <c r="J24" s="54"/>
-      <c r="K24" s="102"/>
+      <c r="K24" s="130"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B25" s="103" t="s">
+      <c r="B25" s="128" t="s">
         <v>56</v>
       </c>
       <c r="C25" s="59" t="s">
@@ -2864,15 +2897,15 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="54"/>
-      <c r="J25" s="86" t="s">
+      <c r="J25" s="131" t="s">
         <v>58</v>
       </c>
-      <c r="K25" s="100" t="s">
+      <c r="K25" s="129" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B26" s="103"/>
+      <c r="B26" s="128"/>
       <c r="C26" s="61" t="s">
         <v>59</v>
       </c>
@@ -2882,15 +2915,15 @@
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="54"/>
-      <c r="J26" s="87"/>
-      <c r="K26" s="102"/>
+      <c r="J26" s="114"/>
+      <c r="K26" s="130"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B27" s="30" t="s">
         <v>60</v>
       </c>
       <c r="C27" s="39"/>
-      <c r="D27" s="76"/>
+      <c r="D27" s="75"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -2938,51 +2971,51 @@
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
       <c r="I30" s="18"/>
-      <c r="J30" s="75"/>
+      <c r="J30" s="74"/>
       <c r="K30" s="28"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B31" s="157"/>
+      <c r="B31" s="85"/>
       <c r="C31" s="25"/>
       <c r="D31" s="25"/>
-      <c r="E31" s="81"/>
-      <c r="F31" s="81"/>
-      <c r="G31" s="81"/>
-      <c r="H31" s="81"/>
-      <c r="I31" s="81"/>
-      <c r="J31" s="81"/>
-      <c r="K31" s="158"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="80"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="86"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B32" s="157"/>
+      <c r="B32" s="85"/>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
-      <c r="G32" s="81"/>
-      <c r="H32" s="81"/>
-      <c r="I32" s="81"/>
-      <c r="J32" s="81"/>
-      <c r="K32" s="158"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="86"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B33" s="157"/>
+      <c r="B33" s="85"/>
       <c r="C33" s="25"/>
       <c r="D33" s="25"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
-      <c r="G33" s="81"/>
-      <c r="H33" s="81"/>
-      <c r="I33" s="81"/>
-      <c r="J33" s="81"/>
-      <c r="K33" s="158"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="86"/>
     </row>
     <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="119" t="s">
+      <c r="A35" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="111" t="s">
+      <c r="B35" s="134" t="s">
         <v>64</v>
       </c>
       <c r="C35" s="47" t="s">
@@ -3007,14 +3040,14 @@
       <c r="O35" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="P35" s="124" t="s">
+      <c r="P35" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="Q35" s="125"/>
+      <c r="Q35" s="110"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A36" s="120"/>
-      <c r="B36" s="92"/>
+      <c r="A36" s="107"/>
+      <c r="B36" s="127"/>
       <c r="C36" s="53" t="s">
         <v>68</v>
       </c>
@@ -3037,13 +3070,13 @@
       <c r="O36" s="19">
         <v>0</v>
       </c>
-      <c r="P36" s="126" t="s">
+      <c r="P36" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="Q36" s="127"/>
+      <c r="Q36" s="112"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A37" s="120"/>
+      <c r="A37" s="107"/>
       <c r="B37" s="29" t="s">
         <v>70</v>
       </c>
@@ -3052,14 +3085,14 @@
       </c>
       <c r="D37" s="41"/>
       <c r="E37" s="51"/>
-      <c r="F37" s="139" t="s">
+      <c r="F37" s="124" t="s">
         <v>72</v>
       </c>
-      <c r="G37" s="140"/>
-      <c r="H37" s="141"/>
+      <c r="G37" s="125"/>
+      <c r="H37" s="126"/>
       <c r="I37" s="50"/>
       <c r="J37" s="42"/>
-      <c r="K37" s="77"/>
+      <c r="K37" s="76"/>
       <c r="M37" s="13">
         <v>0</v>
       </c>
@@ -3069,13 +3102,13 @@
       <c r="O37" s="10">
         <v>1</v>
       </c>
-      <c r="P37" s="122" t="s">
+      <c r="P37" s="99" t="s">
         <v>106</v>
       </c>
-      <c r="Q37" s="123"/>
+      <c r="Q37" s="101"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A38" s="120"/>
+      <c r="A38" s="107"/>
       <c r="B38" s="30" t="s">
         <v>73</v>
       </c>
@@ -3103,28 +3136,28 @@
       <c r="O38" s="10">
         <v>0</v>
       </c>
-      <c r="P38" s="122" t="s">
+      <c r="P38" s="99" t="s">
         <v>107</v>
       </c>
-      <c r="Q38" s="123"/>
+      <c r="Q38" s="101"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A39" s="120"/>
-      <c r="B39" s="92" t="s">
+      <c r="A39" s="107"/>
+      <c r="B39" s="127" t="s">
         <v>75</v>
       </c>
       <c r="C39" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="147" t="s">
+      <c r="D39" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="E39" s="148"/>
-      <c r="F39" s="148"/>
-      <c r="G39" s="148"/>
-      <c r="H39" s="148"/>
-      <c r="I39" s="149"/>
-      <c r="J39" s="78"/>
+      <c r="E39" s="91"/>
+      <c r="F39" s="91"/>
+      <c r="G39" s="91"/>
+      <c r="H39" s="91"/>
+      <c r="I39" s="92"/>
+      <c r="J39" s="77"/>
       <c r="K39" s="22" t="s">
         <v>41</v>
       </c>
@@ -3137,24 +3170,24 @@
       <c r="O39" s="10">
         <v>1</v>
       </c>
-      <c r="P39" s="122" t="s">
+      <c r="P39" s="99" t="s">
         <v>108</v>
       </c>
-      <c r="Q39" s="123"/>
+      <c r="Q39" s="101"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A40" s="120"/>
-      <c r="B40" s="92"/>
+      <c r="A40" s="107"/>
+      <c r="B40" s="127"/>
       <c r="C40" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="150"/>
-      <c r="E40" s="151"/>
-      <c r="F40" s="151"/>
-      <c r="G40" s="151"/>
-      <c r="H40" s="151"/>
-      <c r="I40" s="152"/>
-      <c r="J40" s="79"/>
+      <c r="D40" s="93"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="94"/>
+      <c r="G40" s="94"/>
+      <c r="H40" s="94"/>
+      <c r="I40" s="95"/>
+      <c r="J40" s="78"/>
       <c r="K40" s="22" t="s">
         <v>69</v>
       </c>
@@ -3167,24 +3200,24 @@
       <c r="O40" s="10">
         <v>0</v>
       </c>
-      <c r="P40" s="122" t="s">
+      <c r="P40" s="99" t="s">
         <v>109</v>
       </c>
-      <c r="Q40" s="123"/>
+      <c r="Q40" s="101"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A41" s="120"/>
-      <c r="B41" s="92"/>
+      <c r="A41" s="107"/>
+      <c r="B41" s="127"/>
       <c r="C41" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="132"/>
-      <c r="E41" s="133"/>
-      <c r="F41" s="133"/>
-      <c r="G41" s="133"/>
-      <c r="H41" s="133"/>
-      <c r="I41" s="134"/>
-      <c r="J41" s="80"/>
+      <c r="D41" s="96"/>
+      <c r="E41" s="97"/>
+      <c r="F41" s="97"/>
+      <c r="G41" s="97"/>
+      <c r="H41" s="97"/>
+      <c r="I41" s="98"/>
+      <c r="J41" s="79"/>
       <c r="K41" s="52"/>
       <c r="M41" s="13">
         <v>1</v>
@@ -3195,14 +3228,14 @@
       <c r="O41" s="10">
         <v>1</v>
       </c>
-      <c r="P41" s="122" t="s">
+      <c r="P41" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="Q41" s="123"/>
+      <c r="Q41" s="101"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A42" s="120"/>
-      <c r="B42" s="118" t="s">
+      <c r="A42" s="107"/>
+      <c r="B42" s="121" t="s">
         <v>80</v>
       </c>
       <c r="C42" s="48" t="s">
@@ -3227,14 +3260,14 @@
       <c r="O42" s="10">
         <v>0</v>
       </c>
-      <c r="P42" s="122" t="s">
+      <c r="P42" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="Q42" s="123"/>
+      <c r="Q42" s="101"/>
     </row>
     <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="120"/>
-      <c r="B43" s="118"/>
+      <c r="A43" s="107"/>
+      <c r="B43" s="121"/>
       <c r="C43" s="55" t="s">
         <v>83</v>
       </c>
@@ -3257,13 +3290,13 @@
       <c r="O43" s="18">
         <v>1</v>
       </c>
-      <c r="P43" s="142" t="s">
+      <c r="P43" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="Q43" s="144"/>
+      <c r="Q43" s="89"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A44" s="120"/>
+      <c r="A44" s="107"/>
       <c r="B44" s="30" t="s">
         <v>84</v>
       </c>
@@ -3278,7 +3311,7 @@
       <c r="K44" s="26"/>
     </row>
     <row r="45" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="121"/>
+      <c r="A45" s="108"/>
       <c r="B45" s="31" t="s">
         <v>85</v>
       </c>
@@ -3294,25 +3327,25 @@
     </row>
     <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="47" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="119" t="s">
+      <c r="A47" s="106" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="137" t="s">
+      <c r="B47" s="122" t="s">
         <v>89</v>
       </c>
       <c r="C47" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="129" t="s">
+      <c r="D47" s="115" t="s">
         <v>88</v>
       </c>
-      <c r="E47" s="130"/>
-      <c r="F47" s="131"/>
-      <c r="G47" s="135" t="s">
+      <c r="E47" s="116"/>
+      <c r="F47" s="117"/>
+      <c r="G47" s="118" t="s">
         <v>90</v>
       </c>
       <c r="H47" s="64"/>
-      <c r="I47" s="128" t="s">
+      <c r="I47" s="113" t="s">
         <v>91</v>
       </c>
       <c r="J47" s="19"/>
@@ -3323,44 +3356,44 @@
       <c r="N47" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="O47" s="153" t="s">
+      <c r="O47" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="P47" s="154"/>
-      <c r="Q47" s="155"/>
+      <c r="P47" s="103"/>
+      <c r="Q47" s="104"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A48" s="120"/>
-      <c r="B48" s="138"/>
+      <c r="A48" s="107"/>
+      <c r="B48" s="123"/>
       <c r="C48" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="D48" s="132"/>
-      <c r="E48" s="133"/>
-      <c r="F48" s="134"/>
-      <c r="G48" s="117"/>
+      <c r="D48" s="96"/>
+      <c r="E48" s="97"/>
+      <c r="F48" s="98"/>
+      <c r="G48" s="119"/>
       <c r="H48" s="44"/>
-      <c r="I48" s="87"/>
-      <c r="J48" s="72"/>
-      <c r="K48" s="73"/>
+      <c r="I48" s="114"/>
+      <c r="J48" s="71"/>
+      <c r="K48" s="72"/>
       <c r="M48" s="13">
         <v>0</v>
       </c>
       <c r="N48" s="10">
         <v>0</v>
       </c>
-      <c r="O48" s="122" t="s">
+      <c r="O48" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="P48" s="109"/>
-      <c r="Q48" s="123"/>
+      <c r="P48" s="100"/>
+      <c r="Q48" s="101"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A49" s="120"/>
-      <c r="B49" s="118" t="s">
+      <c r="A49" s="107"/>
+      <c r="B49" s="121" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="136" t="s">
+      <c r="C49" s="120" t="s">
         <v>95</v>
       </c>
       <c r="D49" s="25"/>
@@ -3369,8 +3402,8 @@
       <c r="G49" s="17"/>
       <c r="H49" s="17"/>
       <c r="I49" s="17"/>
-      <c r="J49" s="74"/>
-      <c r="K49" s="156" t="s">
+      <c r="J49" s="73"/>
+      <c r="K49" s="105" t="s">
         <v>96</v>
       </c>
       <c r="M49" s="13">
@@ -3379,45 +3412,45 @@
       <c r="N49" s="10">
         <v>1</v>
       </c>
-      <c r="O49" s="122" t="s">
+      <c r="O49" s="99" t="s">
         <v>115</v>
       </c>
-      <c r="P49" s="109"/>
-      <c r="Q49" s="123"/>
+      <c r="P49" s="100"/>
+      <c r="Q49" s="101"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A50" s="120"/>
-      <c r="B50" s="118"/>
-      <c r="C50" s="136"/>
-      <c r="D50" s="76"/>
+      <c r="A50" s="107"/>
+      <c r="B50" s="121"/>
+      <c r="C50" s="120"/>
+      <c r="D50" s="75"/>
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
       <c r="G50" s="17"/>
       <c r="H50" s="17"/>
       <c r="I50" s="17"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="156"/>
+      <c r="J50" s="73"/>
+      <c r="K50" s="105"/>
       <c r="M50" s="13">
         <v>1</v>
       </c>
       <c r="N50" s="10">
         <v>0</v>
       </c>
-      <c r="O50" s="122" t="s">
+      <c r="O50" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="P50" s="109"/>
-      <c r="Q50" s="123"/>
+      <c r="P50" s="100"/>
+      <c r="Q50" s="101"/>
     </row>
     <row r="51" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="120"/>
+      <c r="A51" s="107"/>
       <c r="B51" s="36" t="s">
         <v>97</v>
       </c>
       <c r="C51" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="D51" s="82"/>
+      <c r="D51" s="81"/>
       <c r="E51" s="38"/>
       <c r="F51" s="38"/>
       <c r="G51" s="38"/>
@@ -3431,14 +3464,14 @@
       <c r="N51" s="18">
         <v>1</v>
       </c>
-      <c r="O51" s="142" t="s">
+      <c r="O51" s="87" t="s">
         <v>117</v>
       </c>
-      <c r="P51" s="143"/>
-      <c r="Q51" s="144"/>
+      <c r="P51" s="88"/>
+      <c r="Q51" s="89"/>
     </row>
     <row r="52" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="121"/>
+      <c r="A52" s="108"/>
       <c r="B52" s="34" t="s">
         <v>102</v>
       </c>
@@ -3454,20 +3487,44 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="O51:Q51"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="D39:I41"/>
-    <mergeCell ref="P43:Q43"/>
-    <mergeCell ref="O49:Q49"/>
-    <mergeCell ref="O47:Q47"/>
-    <mergeCell ref="O48:Q48"/>
-    <mergeCell ref="O50:Q50"/>
-    <mergeCell ref="K49:K50"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="O14:Q14"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="E3:E9"/>
+    <mergeCell ref="F3:I9"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F14:H15"/>
+    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="K10:K13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:G13"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="A35:A45"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="J25:J26"/>
     <mergeCell ref="A47:A52"/>
     <mergeCell ref="P40:Q40"/>
     <mergeCell ref="P39:Q39"/>
@@ -3484,44 +3541,20 @@
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="A35:A45"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="J18:J20"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F14:H15"/>
-    <mergeCell ref="J10:J13"/>
-    <mergeCell ref="K10:K13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:G13"/>
-    <mergeCell ref="I10:I13"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="F3:I4"/>
-    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="O51:Q51"/>
+    <mergeCell ref="D39:I41"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="O49:Q49"/>
+    <mergeCell ref="O47:Q47"/>
+    <mergeCell ref="O48:Q48"/>
+    <mergeCell ref="O50:Q50"/>
+    <mergeCell ref="K49:K50"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="K3:K9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>